<commit_message>
attempt to create relationship
</commit_message>
<xml_diff>
--- a/seed_data.xlsx
+++ b/seed_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\EPFC\2324\PRBD\PRBD2324\tutos\projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB32231-A881-4281-9A5B-6B066EB8C75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB475D29-7146-4989-AD17-985481B9215E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{1476758A-0B9A-44C3-B34C-9348D635B8CF}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="15943" activeTab="1" xr2:uid="{1476758A-0B9A-44C3-B34C-9348D635B8CF}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -231,12 +231,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -251,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -274,20 +280,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="37">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -361,6 +361,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -434,6 +437,12 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -481,89 +490,89 @@
   <autoFilter ref="A1:E6" xr:uid="{805EC10E-4DE0-499A-A014-91B0B5052EC9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B66FF063-0899-4FD2-ACE0-D009376E9692}" name="id" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{E77E58A2-8CCE-4D72-995A-D872739161F9}" name="email" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{26E46A6A-714B-4ABB-A580-98C1E43D8E35}" name="hashed_password" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{14CD761B-A946-433E-9672-E78405672D26}" name="full_name" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{0C6E7B60-35B7-41B5-8DEF-3B76228582E3}" name="role" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{E77E58A2-8CCE-4D72-995A-D872739161F9}" name="email" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{26E46A6A-714B-4ABB-A580-98C1E43D8E35}" name="hashed_password" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{14CD761B-A946-433E-9672-E78405672D26}" name="full_name" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{0C6E7B60-35B7-41B5-8DEF-3B76228582E3}" name="role" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F46F2DDB-EE63-4CA8-86BE-7BF2A7A2D5F0}" name="Table2" displayName="Table2" ref="A1:E6" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F46F2DDB-EE63-4CA8-86BE-7BF2A7A2D5F0}" name="Table2" displayName="Table2" ref="A1:E6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:E6" xr:uid="{F46F2DDB-EE63-4CA8-86BE-7BF2A7A2D5F0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D8D9A886-A58D-4E61-86DF-33B88F98D643}" name="id" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{5E7B0066-9971-4CF1-A24B-5FF311476AF5}" name="title" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{2EC05261-1616-41B1-BDCA-6FC87E0791C9}" name="description" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{6961F688-1975-43B2-B8D0-8835354E1DA9}" name="created_at" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{25546971-2451-49AF-A05F-AC12920CF37C}" name="creator" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{D8D9A886-A58D-4E61-86DF-33B88F98D643}" name="id" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{5E7B0066-9971-4CF1-A24B-5FF311476AF5}" name="title" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{2EC05261-1616-41B1-BDCA-6FC87E0791C9}" name="description" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{6961F688-1975-43B2-B8D0-8835354E1DA9}" name="created_at" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{25546971-2451-49AF-A05F-AC12920CF37C}" name="creator" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{508FD46A-E2B0-470B-B0E3-AB87FA4F5CF3}" name="Table3" displayName="Table3" ref="A1:B15" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{508FD46A-E2B0-470B-B0E3-AB87FA4F5CF3}" name="Table3" displayName="Table3" ref="A1:B15" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:B15" xr:uid="{508FD46A-E2B0-470B-B0E3-AB87FA4F5CF3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{936F4877-9115-4CAB-941C-CF2525B1646E}" name="user" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{7165F0E3-04DA-4717-9EF0-A22FEF6CB374}" name="tricount" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{936F4877-9115-4CAB-941C-CF2525B1646E}" name="user" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{7165F0E3-04DA-4717-9EF0-A22FEF6CB374}" name="tricount" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2155495-F6A8-4F45-AC5A-4F2AED5E6AFE}" name="Table4" displayName="Table4" ref="A1:F12" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2155495-F6A8-4F45-AC5A-4F2AED5E6AFE}" name="Table4" displayName="Table4" ref="A1:F12" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A1:F12" xr:uid="{D2155495-F6A8-4F45-AC5A-4F2AED5E6AFE}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A243B9F9-42A2-4198-A496-62BCC412D678}" name="id" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{A243B9F9-42A2-4198-A496-62BCC412D678}" name="id" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{D06BB176-DF8C-4D93-BD9D-4C4FC28719E1}" name="title"/>
-    <tableColumn id="5" xr3:uid="{97BF38BD-1FE1-416F-93C5-170315C269D0}" name="tricount" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{F1F307EA-46CC-4D1D-9681-F6EC3FBA547E}" name="amount" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{23217D1A-B185-44EC-885A-517429C6DEA5}" name="operation_date" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{4088A7B6-9295-46CE-82A3-EC9E18195369}" name="initiator" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{97BF38BD-1FE1-416F-93C5-170315C269D0}" name="tricount" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{F1F307EA-46CC-4D1D-9681-F6EC3FBA547E}" name="amount" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{23217D1A-B185-44EC-885A-517429C6DEA5}" name="operation_date" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{4088A7B6-9295-46CE-82A3-EC9E18195369}" name="initiator" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E3224914-E6E9-45D3-A06C-F03166C73119}" name="Table5" displayName="Table5" ref="A1:C27" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E3224914-E6E9-45D3-A06C-F03166C73119}" name="Table5" displayName="Table5" ref="A1:C27" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:C27" xr:uid="{E3224914-E6E9-45D3-A06C-F03166C73119}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{76D85872-402A-43FE-8F6F-DCB6AA1BBC44}" name="operation" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{815183E6-C664-4136-B3CD-FE0AA152C83F}" name="user" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{CF94AAA1-A4B8-4F1F-9B38-6F0DEEE2C64E}" name="weight" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{76D85872-402A-43FE-8F6F-DCB6AA1BBC44}" name="operation" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{815183E6-C664-4136-B3CD-FE0AA152C83F}" name="user" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{CF94AAA1-A4B8-4F1F-9B38-6F0DEEE2C64E}" name="weight" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2399594E-798C-4EA6-A6BD-6FFED77EF3EC}" name="Table6" displayName="Table6" ref="A1:C3" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2399594E-798C-4EA6-A6BD-6FFED77EF3EC}" name="Table6" displayName="Table6" ref="A1:C3" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:C3" xr:uid="{2399594E-798C-4EA6-A6BD-6FFED77EF3EC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C3">
     <sortCondition ref="A1:A3"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BE1AD935-CDA6-4921-8829-36AD5138F7CA}" name="id" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{BE1AD935-CDA6-4921-8829-36AD5138F7CA}" name="id" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{F5408C19-7C7E-4FFC-A3C2-7686B58250F4}" name="title"/>
-    <tableColumn id="3" xr3:uid="{36F46884-6D2E-4FE1-B198-E4E2B00A64C6}" name="tricount" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{36F46884-6D2E-4FE1-B198-E4E2B00A64C6}" name="tricount" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{26512D55-0987-4DED-9672-12AAF7657A5D}" name="Table7" displayName="Table7" ref="A1:C6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{26512D55-0987-4DED-9672-12AAF7657A5D}" name="Table7" displayName="Table7" ref="A1:C6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C6" xr:uid="{26512D55-0987-4DED-9672-12AAF7657A5D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5DAFA872-5E84-46C7-AD7E-AD479FF39160}" name="template" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{DE1AA840-DFFA-46B4-9064-D54060A3BFCD}" name="user" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{0F306DB1-3632-4D09-AA0B-03E875807AC1}" name="weight" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{5DAFA872-5E84-46C7-AD7E-AD479FF39160}" name="template" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{DE1AA840-DFFA-46B4-9064-D54060A3BFCD}" name="user" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{0F306DB1-3632-4D09-AA0B-03E875807AC1}" name="weight" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -888,22 +897,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7495DE-440D-41BB-8577-CAA8980A2511}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.3984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.46484375" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.1328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.3828125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.4609375" customWidth="1"/>
+    <col min="4" max="4" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.15234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -920,7 +929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -937,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -954,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -971,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -988,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1018,21 +1027,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26BCE26-BAF0-4E09-84B8-4C4AB7F57209}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.3984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.3828125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.23046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3046875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="8.69140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1064,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1079,7 +1088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>4</v>
       </c>
@@ -1096,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -1113,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>6</v>
       </c>
@@ -1123,8 +1132,8 @@
       <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="7">
-        <v>45109.770972222221</v>
+      <c r="D6" s="8">
+        <v>45079.770972222221</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -1147,12 +1156,12 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="3"/>
+    <col min="1" max="2" width="9.07421875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1160,7 +1169,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1168,7 +1177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1176,7 +1185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1184,7 +1193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1192,7 +1201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1200,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>2</v>
       </c>
@@ -1208,7 +1217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -1216,7 +1225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -1224,7 +1233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -1232,7 +1241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -1240,7 +1249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>3</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>4</v>
       </c>
@@ -1256,7 +1265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>4</v>
       </c>
@@ -1264,7 +1273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>4</v>
       </c>
@@ -1290,17 +1299,17 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="3"/>
-    <col min="2" max="2" width="17.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.07421875" style="3"/>
+    <col min="2" max="2" width="17.53515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3828125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.61328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1320,7 +1329,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1341,7 +1350,7 @@
       </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1362,7 +1371,7 @@
       </c>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1383,7 +1392,7 @@
       </c>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1404,7 +1413,7 @@
       </c>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1425,7 +1434,7 @@
       </c>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1446,7 +1455,7 @@
       </c>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1467,7 +1476,7 @@
       </c>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1488,7 +1497,7 @@
       </c>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1509,7 +1518,7 @@
       </c>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1530,7 +1539,7 @@
       </c>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1568,14 +1577,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -1586,7 +1595,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1597,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1608,7 +1617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1619,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1630,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1641,7 +1650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1652,7 +1661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>3</v>
       </c>
@@ -1663,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>4</v>
       </c>
@@ -1674,7 +1683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>4</v>
       </c>
@@ -1685,7 +1694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>4</v>
       </c>
@@ -1696,7 +1705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>5</v>
       </c>
@@ -1707,7 +1716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>5</v>
       </c>
@@ -1718,7 +1727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>5</v>
       </c>
@@ -1729,7 +1738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>6</v>
       </c>
@@ -1740,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>6</v>
       </c>
@@ -1751,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>7</v>
       </c>
@@ -1762,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>7</v>
       </c>
@@ -1773,7 +1782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>7</v>
       </c>
@@ -1784,7 +1793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>8</v>
       </c>
@@ -1795,7 +1804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>8</v>
       </c>
@@ -1806,7 +1815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>9</v>
       </c>
@@ -1817,7 +1826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>9</v>
       </c>
@@ -1828,7 +1837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>10</v>
       </c>
@@ -1839,7 +1848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>10</v>
       </c>
@@ -1850,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>11</v>
       </c>
@@ -1861,7 +1870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>11</v>
       </c>
@@ -1889,14 +1898,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.46484375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.4609375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.4609375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1907,7 +1916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1918,7 +1927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1946,14 +1955,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1964,7 +1973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1975,7 +1984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1986,7 +1995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1997,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -2008,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>2</v>
       </c>

</xml_diff>